<commit_message>
updates metadata sheet and start processing data
this commit:
* updates the spreadsheet for metadata by filling
out more examples in the attributes sheet
* creates and starts cleaning the data table for this
data package
</commit_message>
<xml_diff>
--- a/inst/extdata/metadata-creation-template/example/example-metadata.xlsx
+++ b/inst/extdata/metadata-creation-template/example/example-metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuel\Documents\metadata-creation-template\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emanuel\Projects\cvpia\EDIutils\inst\extdata\metadata-creation-template\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB63B92C-D189-475F-A2F0-4A7A5EAD52BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3134CCD-1CE9-41C9-AB86-A144A681EC7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="500" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="taxonomic_coverage" sheetId="8" r:id="rId8"/>
     <sheet name="attribute" sheetId="9" r:id="rId9"/>
     <sheet name="code_definitions" sheetId="10" r:id="rId10"/>
-    <sheet name="_lookups" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="165">
   <si>
     <t>first_name</t>
   </si>
@@ -524,6 +523,12 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>estimated flow in cubic feet per second</t>
+  </si>
+  <si>
+    <t>interger</t>
   </si>
 </sst>
 </file>
@@ -602,113 +607,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1193,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1393,18 +1292,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB49137-AB3C-4126-ACB1-21C34426AD86}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1756,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2106,6 +1993,9 @@
       <c r="D15" s="3" t="s">
         <v>130</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="I15" s="3" t="s">
         <v>130</v>
       </c>
@@ -2135,6 +2025,9 @@
       <c r="D16" s="3" t="s">
         <v>130</v>
       </c>
+      <c r="F16" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="I16" s="3" t="s">
         <v>130</v>
       </c>
@@ -2164,6 +2057,9 @@
       <c r="D17" s="3" t="s">
         <v>130</v>
       </c>
+      <c r="F17" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="I17" s="3" t="s">
         <v>130</v>
       </c>
@@ -2193,6 +2089,9 @@
       <c r="D18" s="3" t="s">
         <v>130</v>
       </c>
+      <c r="F18" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="I18" s="3" t="s">
         <v>130</v>
       </c>
@@ -2213,20 +2112,50 @@
       <c r="A19" s="3" t="s">
         <v>118</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>119</v>
       </c>
+      <c r="B20" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>121</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>10000000</v>
       </c>
     </row>
   </sheetData>
@@ -2241,7 +2170,7 @@
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{2BC30EC9-2402-4CAD-96D7-4D4098E00DE7}">
-      <formula1>"natural,whole,interget,real"</formula1>
+      <formula1>"natural,whole,interger,real"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{5F281007-CBDB-4DAC-AD0E-296D46D22A6E}">
       <formula1>"ratio,interval"</formula1>

</xml_diff>

<commit_message>
adds more processing to fix factors and units
</commit_message>
<xml_diff>
--- a/inst/extdata/metadata-creation-template/example/example-metadata.xlsx
+++ b/inst/extdata/metadata-creation-template/example/example-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emanuel\Projects\cvpia\EDIutils\inst\extdata\metadata-creation-template\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3134CCD-1CE9-41C9-AB86-A144A681EC7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361EE11A-9A10-4C18-A6AD-9705B5357BF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,17 @@
     <sheet name="attribute" sheetId="9" r:id="rId9"/>
     <sheet name="code_definitions" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -34,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="168">
   <si>
     <t>first_name</t>
   </si>
@@ -438,15 +447,6 @@
     <t>indicates what treatment type was used for comparison</t>
   </si>
   <si>
-    <t>Impact</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
-    <t>Baseline</t>
-  </si>
-  <si>
     <t>existing area used for comparison</t>
   </si>
   <si>
@@ -529,13 +529,31 @@
   </si>
   <si>
     <t>interger</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>observer</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>impact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -565,6 +583,13 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -587,7 +612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,6 +627,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1090,14 +1119,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="25.125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
@@ -1179,12 +1209,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
         <v>106</v>
@@ -1192,10 +1222,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
         <v>106</v>
@@ -1203,90 +1233,95 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
+      <c r="A11" t="s">
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
+      <c r="A12" t="s">
+        <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3</v>
+      <c r="A13" t="s">
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>4</v>
+      <c r="A14" t="s">
+        <v>147</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
+      <c r="A15" t="s">
+        <v>148</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0</v>
+      <c r="A16" t="s">
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
+      <c r="A17" t="s">
+        <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1644,7 +1679,7 @@
   <dimension ref="A1:AMJ22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1652,57 +1687,1065 @@
     <col min="1" max="1024" width="19.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1024" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="8"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="8"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
+      <c r="CC1" s="8"/>
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="8"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="8"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="8"/>
+      <c r="CJ1" s="8"/>
+      <c r="CK1" s="8"/>
+      <c r="CL1" s="8"/>
+      <c r="CM1" s="8"/>
+      <c r="CN1" s="8"/>
+      <c r="CO1" s="8"/>
+      <c r="CP1" s="8"/>
+      <c r="CQ1" s="8"/>
+      <c r="CR1" s="8"/>
+      <c r="CS1" s="8"/>
+      <c r="CT1" s="8"/>
+      <c r="CU1" s="8"/>
+      <c r="CV1" s="8"/>
+      <c r="CW1" s="8"/>
+      <c r="CX1" s="8"/>
+      <c r="CY1" s="8"/>
+      <c r="CZ1" s="8"/>
+      <c r="DA1" s="8"/>
+      <c r="DB1" s="8"/>
+      <c r="DC1" s="8"/>
+      <c r="DD1" s="8"/>
+      <c r="DE1" s="8"/>
+      <c r="DF1" s="8"/>
+      <c r="DG1" s="8"/>
+      <c r="DH1" s="8"/>
+      <c r="DI1" s="8"/>
+      <c r="DJ1" s="8"/>
+      <c r="DK1" s="8"/>
+      <c r="DL1" s="8"/>
+      <c r="DM1" s="8"/>
+      <c r="DN1" s="8"/>
+      <c r="DO1" s="8"/>
+      <c r="DP1" s="8"/>
+      <c r="DQ1" s="8"/>
+      <c r="DR1" s="8"/>
+      <c r="DS1" s="8"/>
+      <c r="DT1" s="8"/>
+      <c r="DU1" s="8"/>
+      <c r="DV1" s="8"/>
+      <c r="DW1" s="8"/>
+      <c r="DX1" s="8"/>
+      <c r="DY1" s="8"/>
+      <c r="DZ1" s="8"/>
+      <c r="EA1" s="8"/>
+      <c r="EB1" s="8"/>
+      <c r="EC1" s="8"/>
+      <c r="ED1" s="8"/>
+      <c r="EE1" s="8"/>
+      <c r="EF1" s="8"/>
+      <c r="EG1" s="8"/>
+      <c r="EH1" s="8"/>
+      <c r="EI1" s="8"/>
+      <c r="EJ1" s="8"/>
+      <c r="EK1" s="8"/>
+      <c r="EL1" s="8"/>
+      <c r="EM1" s="8"/>
+      <c r="EN1" s="8"/>
+      <c r="EO1" s="8"/>
+      <c r="EP1" s="8"/>
+      <c r="EQ1" s="8"/>
+      <c r="ER1" s="8"/>
+      <c r="ES1" s="8"/>
+      <c r="ET1" s="8"/>
+      <c r="EU1" s="8"/>
+      <c r="EV1" s="8"/>
+      <c r="EW1" s="8"/>
+      <c r="EX1" s="8"/>
+      <c r="EY1" s="8"/>
+      <c r="EZ1" s="8"/>
+      <c r="FA1" s="8"/>
+      <c r="FB1" s="8"/>
+      <c r="FC1" s="8"/>
+      <c r="FD1" s="8"/>
+      <c r="FE1" s="8"/>
+      <c r="FF1" s="8"/>
+      <c r="FG1" s="8"/>
+      <c r="FH1" s="8"/>
+      <c r="FI1" s="8"/>
+      <c r="FJ1" s="8"/>
+      <c r="FK1" s="8"/>
+      <c r="FL1" s="8"/>
+      <c r="FM1" s="8"/>
+      <c r="FN1" s="8"/>
+      <c r="FO1" s="8"/>
+      <c r="FP1" s="8"/>
+      <c r="FQ1" s="8"/>
+      <c r="FR1" s="8"/>
+      <c r="FS1" s="8"/>
+      <c r="FT1" s="8"/>
+      <c r="FU1" s="8"/>
+      <c r="FV1" s="8"/>
+      <c r="FW1" s="8"/>
+      <c r="FX1" s="8"/>
+      <c r="FY1" s="8"/>
+      <c r="FZ1" s="8"/>
+      <c r="GA1" s="8"/>
+      <c r="GB1" s="8"/>
+      <c r="GC1" s="8"/>
+      <c r="GD1" s="8"/>
+      <c r="GE1" s="8"/>
+      <c r="GF1" s="8"/>
+      <c r="GG1" s="8"/>
+      <c r="GH1" s="8"/>
+      <c r="GI1" s="8"/>
+      <c r="GJ1" s="8"/>
+      <c r="GK1" s="8"/>
+      <c r="GL1" s="8"/>
+      <c r="GM1" s="8"/>
+      <c r="GN1" s="8"/>
+      <c r="GO1" s="8"/>
+      <c r="GP1" s="8"/>
+      <c r="GQ1" s="8"/>
+      <c r="GR1" s="8"/>
+      <c r="GS1" s="8"/>
+      <c r="GT1" s="8"/>
+      <c r="GU1" s="8"/>
+      <c r="GV1" s="8"/>
+      <c r="GW1" s="8"/>
+      <c r="GX1" s="8"/>
+      <c r="GY1" s="8"/>
+      <c r="GZ1" s="8"/>
+      <c r="HA1" s="8"/>
+      <c r="HB1" s="8"/>
+      <c r="HC1" s="8"/>
+      <c r="HD1" s="8"/>
+      <c r="HE1" s="8"/>
+      <c r="HF1" s="8"/>
+      <c r="HG1" s="8"/>
+      <c r="HH1" s="8"/>
+      <c r="HI1" s="8"/>
+      <c r="HJ1" s="8"/>
+      <c r="HK1" s="8"/>
+      <c r="HL1" s="8"/>
+      <c r="HM1" s="8"/>
+      <c r="HN1" s="8"/>
+      <c r="HO1" s="8"/>
+      <c r="HP1" s="8"/>
+      <c r="HQ1" s="8"/>
+      <c r="HR1" s="8"/>
+      <c r="HS1" s="8"/>
+      <c r="HT1" s="8"/>
+      <c r="HU1" s="8"/>
+      <c r="HV1" s="8"/>
+      <c r="HW1" s="8"/>
+      <c r="HX1" s="8"/>
+      <c r="HY1" s="8"/>
+      <c r="HZ1" s="8"/>
+      <c r="IA1" s="8"/>
+      <c r="IB1" s="8"/>
+      <c r="IC1" s="8"/>
+      <c r="ID1" s="8"/>
+      <c r="IE1" s="8"/>
+      <c r="IF1" s="8"/>
+      <c r="IG1" s="8"/>
+      <c r="IH1" s="8"/>
+      <c r="II1" s="8"/>
+      <c r="IJ1" s="8"/>
+      <c r="IK1" s="8"/>
+      <c r="IL1" s="8"/>
+      <c r="IM1" s="8"/>
+      <c r="IN1" s="8"/>
+      <c r="IO1" s="8"/>
+      <c r="IP1" s="8"/>
+      <c r="IQ1" s="8"/>
+      <c r="IR1" s="8"/>
+      <c r="IS1" s="8"/>
+      <c r="IT1" s="8"/>
+      <c r="IU1" s="8"/>
+      <c r="IV1" s="8"/>
+      <c r="IW1" s="8"/>
+      <c r="IX1" s="8"/>
+      <c r="IY1" s="8"/>
+      <c r="IZ1" s="8"/>
+      <c r="JA1" s="8"/>
+      <c r="JB1" s="8"/>
+      <c r="JC1" s="8"/>
+      <c r="JD1" s="8"/>
+      <c r="JE1" s="8"/>
+      <c r="JF1" s="8"/>
+      <c r="JG1" s="8"/>
+      <c r="JH1" s="8"/>
+      <c r="JI1" s="8"/>
+      <c r="JJ1" s="8"/>
+      <c r="JK1" s="8"/>
+      <c r="JL1" s="8"/>
+      <c r="JM1" s="8"/>
+      <c r="JN1" s="8"/>
+      <c r="JO1" s="8"/>
+      <c r="JP1" s="8"/>
+      <c r="JQ1" s="8"/>
+      <c r="JR1" s="8"/>
+      <c r="JS1" s="8"/>
+      <c r="JT1" s="8"/>
+      <c r="JU1" s="8"/>
+      <c r="JV1" s="8"/>
+      <c r="JW1" s="8"/>
+      <c r="JX1" s="8"/>
+      <c r="JY1" s="8"/>
+      <c r="JZ1" s="8"/>
+      <c r="KA1" s="8"/>
+      <c r="KB1" s="8"/>
+      <c r="KC1" s="8"/>
+      <c r="KD1" s="8"/>
+      <c r="KE1" s="8"/>
+      <c r="KF1" s="8"/>
+      <c r="KG1" s="8"/>
+      <c r="KH1" s="8"/>
+      <c r="KI1" s="8"/>
+      <c r="KJ1" s="8"/>
+      <c r="KK1" s="8"/>
+      <c r="KL1" s="8"/>
+      <c r="KM1" s="8"/>
+      <c r="KN1" s="8"/>
+      <c r="KO1" s="8"/>
+      <c r="KP1" s="8"/>
+      <c r="KQ1" s="8"/>
+      <c r="KR1" s="8"/>
+      <c r="KS1" s="8"/>
+      <c r="KT1" s="8"/>
+      <c r="KU1" s="8"/>
+      <c r="KV1" s="8"/>
+      <c r="KW1" s="8"/>
+      <c r="KX1" s="8"/>
+      <c r="KY1" s="8"/>
+      <c r="KZ1" s="8"/>
+      <c r="LA1" s="8"/>
+      <c r="LB1" s="8"/>
+      <c r="LC1" s="8"/>
+      <c r="LD1" s="8"/>
+      <c r="LE1" s="8"/>
+      <c r="LF1" s="8"/>
+      <c r="LG1" s="8"/>
+      <c r="LH1" s="8"/>
+      <c r="LI1" s="8"/>
+      <c r="LJ1" s="8"/>
+      <c r="LK1" s="8"/>
+      <c r="LL1" s="8"/>
+      <c r="LM1" s="8"/>
+      <c r="LN1" s="8"/>
+      <c r="LO1" s="8"/>
+      <c r="LP1" s="8"/>
+      <c r="LQ1" s="8"/>
+      <c r="LR1" s="8"/>
+      <c r="LS1" s="8"/>
+      <c r="LT1" s="8"/>
+      <c r="LU1" s="8"/>
+      <c r="LV1" s="8"/>
+      <c r="LW1" s="8"/>
+      <c r="LX1" s="8"/>
+      <c r="LY1" s="8"/>
+      <c r="LZ1" s="8"/>
+      <c r="MA1" s="8"/>
+      <c r="MB1" s="8"/>
+      <c r="MC1" s="8"/>
+      <c r="MD1" s="8"/>
+      <c r="ME1" s="8"/>
+      <c r="MF1" s="8"/>
+      <c r="MG1" s="8"/>
+      <c r="MH1" s="8"/>
+      <c r="MI1" s="8"/>
+      <c r="MJ1" s="8"/>
+      <c r="MK1" s="8"/>
+      <c r="ML1" s="8"/>
+      <c r="MM1" s="8"/>
+      <c r="MN1" s="8"/>
+      <c r="MO1" s="8"/>
+      <c r="MP1" s="8"/>
+      <c r="MQ1" s="8"/>
+      <c r="MR1" s="8"/>
+      <c r="MS1" s="8"/>
+      <c r="MT1" s="8"/>
+      <c r="MU1" s="8"/>
+      <c r="MV1" s="8"/>
+      <c r="MW1" s="8"/>
+      <c r="MX1" s="8"/>
+      <c r="MY1" s="8"/>
+      <c r="MZ1" s="8"/>
+      <c r="NA1" s="8"/>
+      <c r="NB1" s="8"/>
+      <c r="NC1" s="8"/>
+      <c r="ND1" s="8"/>
+      <c r="NE1" s="8"/>
+      <c r="NF1" s="8"/>
+      <c r="NG1" s="8"/>
+      <c r="NH1" s="8"/>
+      <c r="NI1" s="8"/>
+      <c r="NJ1" s="8"/>
+      <c r="NK1" s="8"/>
+      <c r="NL1" s="8"/>
+      <c r="NM1" s="8"/>
+      <c r="NN1" s="8"/>
+      <c r="NO1" s="8"/>
+      <c r="NP1" s="8"/>
+      <c r="NQ1" s="8"/>
+      <c r="NR1" s="8"/>
+      <c r="NS1" s="8"/>
+      <c r="NT1" s="8"/>
+      <c r="NU1" s="8"/>
+      <c r="NV1" s="8"/>
+      <c r="NW1" s="8"/>
+      <c r="NX1" s="8"/>
+      <c r="NY1" s="8"/>
+      <c r="NZ1" s="8"/>
+      <c r="OA1" s="8"/>
+      <c r="OB1" s="8"/>
+      <c r="OC1" s="8"/>
+      <c r="OD1" s="8"/>
+      <c r="OE1" s="8"/>
+      <c r="OF1" s="8"/>
+      <c r="OG1" s="8"/>
+      <c r="OH1" s="8"/>
+      <c r="OI1" s="8"/>
+      <c r="OJ1" s="8"/>
+      <c r="OK1" s="8"/>
+      <c r="OL1" s="8"/>
+      <c r="OM1" s="8"/>
+      <c r="ON1" s="8"/>
+      <c r="OO1" s="8"/>
+      <c r="OP1" s="8"/>
+      <c r="OQ1" s="8"/>
+      <c r="OR1" s="8"/>
+      <c r="OS1" s="8"/>
+      <c r="OT1" s="8"/>
+      <c r="OU1" s="8"/>
+      <c r="OV1" s="8"/>
+      <c r="OW1" s="8"/>
+      <c r="OX1" s="8"/>
+      <c r="OY1" s="8"/>
+      <c r="OZ1" s="8"/>
+      <c r="PA1" s="8"/>
+      <c r="PB1" s="8"/>
+      <c r="PC1" s="8"/>
+      <c r="PD1" s="8"/>
+      <c r="PE1" s="8"/>
+      <c r="PF1" s="8"/>
+      <c r="PG1" s="8"/>
+      <c r="PH1" s="8"/>
+      <c r="PI1" s="8"/>
+      <c r="PJ1" s="8"/>
+      <c r="PK1" s="8"/>
+      <c r="PL1" s="8"/>
+      <c r="PM1" s="8"/>
+      <c r="PN1" s="8"/>
+      <c r="PO1" s="8"/>
+      <c r="PP1" s="8"/>
+      <c r="PQ1" s="8"/>
+      <c r="PR1" s="8"/>
+      <c r="PS1" s="8"/>
+      <c r="PT1" s="8"/>
+      <c r="PU1" s="8"/>
+      <c r="PV1" s="8"/>
+      <c r="PW1" s="8"/>
+      <c r="PX1" s="8"/>
+      <c r="PY1" s="8"/>
+      <c r="PZ1" s="8"/>
+      <c r="QA1" s="8"/>
+      <c r="QB1" s="8"/>
+      <c r="QC1" s="8"/>
+      <c r="QD1" s="8"/>
+      <c r="QE1" s="8"/>
+      <c r="QF1" s="8"/>
+      <c r="QG1" s="8"/>
+      <c r="QH1" s="8"/>
+      <c r="QI1" s="8"/>
+      <c r="QJ1" s="8"/>
+      <c r="QK1" s="8"/>
+      <c r="QL1" s="8"/>
+      <c r="QM1" s="8"/>
+      <c r="QN1" s="8"/>
+      <c r="QO1" s="8"/>
+      <c r="QP1" s="8"/>
+      <c r="QQ1" s="8"/>
+      <c r="QR1" s="8"/>
+      <c r="QS1" s="8"/>
+      <c r="QT1" s="8"/>
+      <c r="QU1" s="8"/>
+      <c r="QV1" s="8"/>
+      <c r="QW1" s="8"/>
+      <c r="QX1" s="8"/>
+      <c r="QY1" s="8"/>
+      <c r="QZ1" s="8"/>
+      <c r="RA1" s="8"/>
+      <c r="RB1" s="8"/>
+      <c r="RC1" s="8"/>
+      <c r="RD1" s="8"/>
+      <c r="RE1" s="8"/>
+      <c r="RF1" s="8"/>
+      <c r="RG1" s="8"/>
+      <c r="RH1" s="8"/>
+      <c r="RI1" s="8"/>
+      <c r="RJ1" s="8"/>
+      <c r="RK1" s="8"/>
+      <c r="RL1" s="8"/>
+      <c r="RM1" s="8"/>
+      <c r="RN1" s="8"/>
+      <c r="RO1" s="8"/>
+      <c r="RP1" s="8"/>
+      <c r="RQ1" s="8"/>
+      <c r="RR1" s="8"/>
+      <c r="RS1" s="8"/>
+      <c r="RT1" s="8"/>
+      <c r="RU1" s="8"/>
+      <c r="RV1" s="8"/>
+      <c r="RW1" s="8"/>
+      <c r="RX1" s="8"/>
+      <c r="RY1" s="8"/>
+      <c r="RZ1" s="8"/>
+      <c r="SA1" s="8"/>
+      <c r="SB1" s="8"/>
+      <c r="SC1" s="8"/>
+      <c r="SD1" s="8"/>
+      <c r="SE1" s="8"/>
+      <c r="SF1" s="8"/>
+      <c r="SG1" s="8"/>
+      <c r="SH1" s="8"/>
+      <c r="SI1" s="8"/>
+      <c r="SJ1" s="8"/>
+      <c r="SK1" s="8"/>
+      <c r="SL1" s="8"/>
+      <c r="SM1" s="8"/>
+      <c r="SN1" s="8"/>
+      <c r="SO1" s="8"/>
+      <c r="SP1" s="8"/>
+      <c r="SQ1" s="8"/>
+      <c r="SR1" s="8"/>
+      <c r="SS1" s="8"/>
+      <c r="ST1" s="8"/>
+      <c r="SU1" s="8"/>
+      <c r="SV1" s="8"/>
+      <c r="SW1" s="8"/>
+      <c r="SX1" s="8"/>
+      <c r="SY1" s="8"/>
+      <c r="SZ1" s="8"/>
+      <c r="TA1" s="8"/>
+      <c r="TB1" s="8"/>
+      <c r="TC1" s="8"/>
+      <c r="TD1" s="8"/>
+      <c r="TE1" s="8"/>
+      <c r="TF1" s="8"/>
+      <c r="TG1" s="8"/>
+      <c r="TH1" s="8"/>
+      <c r="TI1" s="8"/>
+      <c r="TJ1" s="8"/>
+      <c r="TK1" s="8"/>
+      <c r="TL1" s="8"/>
+      <c r="TM1" s="8"/>
+      <c r="TN1" s="8"/>
+      <c r="TO1" s="8"/>
+      <c r="TP1" s="8"/>
+      <c r="TQ1" s="8"/>
+      <c r="TR1" s="8"/>
+      <c r="TS1" s="8"/>
+      <c r="TT1" s="8"/>
+      <c r="TU1" s="8"/>
+      <c r="TV1" s="8"/>
+      <c r="TW1" s="8"/>
+      <c r="TX1" s="8"/>
+      <c r="TY1" s="8"/>
+      <c r="TZ1" s="8"/>
+      <c r="UA1" s="8"/>
+      <c r="UB1" s="8"/>
+      <c r="UC1" s="8"/>
+      <c r="UD1" s="8"/>
+      <c r="UE1" s="8"/>
+      <c r="UF1" s="8"/>
+      <c r="UG1" s="8"/>
+      <c r="UH1" s="8"/>
+      <c r="UI1" s="8"/>
+      <c r="UJ1" s="8"/>
+      <c r="UK1" s="8"/>
+      <c r="UL1" s="8"/>
+      <c r="UM1" s="8"/>
+      <c r="UN1" s="8"/>
+      <c r="UO1" s="8"/>
+      <c r="UP1" s="8"/>
+      <c r="UQ1" s="8"/>
+      <c r="UR1" s="8"/>
+      <c r="US1" s="8"/>
+      <c r="UT1" s="8"/>
+      <c r="UU1" s="8"/>
+      <c r="UV1" s="8"/>
+      <c r="UW1" s="8"/>
+      <c r="UX1" s="8"/>
+      <c r="UY1" s="8"/>
+      <c r="UZ1" s="8"/>
+      <c r="VA1" s="8"/>
+      <c r="VB1" s="8"/>
+      <c r="VC1" s="8"/>
+      <c r="VD1" s="8"/>
+      <c r="VE1" s="8"/>
+      <c r="VF1" s="8"/>
+      <c r="VG1" s="8"/>
+      <c r="VH1" s="8"/>
+      <c r="VI1" s="8"/>
+      <c r="VJ1" s="8"/>
+      <c r="VK1" s="8"/>
+      <c r="VL1" s="8"/>
+      <c r="VM1" s="8"/>
+      <c r="VN1" s="8"/>
+      <c r="VO1" s="8"/>
+      <c r="VP1" s="8"/>
+      <c r="VQ1" s="8"/>
+      <c r="VR1" s="8"/>
+      <c r="VS1" s="8"/>
+      <c r="VT1" s="8"/>
+      <c r="VU1" s="8"/>
+      <c r="VV1" s="8"/>
+      <c r="VW1" s="8"/>
+      <c r="VX1" s="8"/>
+      <c r="VY1" s="8"/>
+      <c r="VZ1" s="8"/>
+      <c r="WA1" s="8"/>
+      <c r="WB1" s="8"/>
+      <c r="WC1" s="8"/>
+      <c r="WD1" s="8"/>
+      <c r="WE1" s="8"/>
+      <c r="WF1" s="8"/>
+      <c r="WG1" s="8"/>
+      <c r="WH1" s="8"/>
+      <c r="WI1" s="8"/>
+      <c r="WJ1" s="8"/>
+      <c r="WK1" s="8"/>
+      <c r="WL1" s="8"/>
+      <c r="WM1" s="8"/>
+      <c r="WN1" s="8"/>
+      <c r="WO1" s="8"/>
+      <c r="WP1" s="8"/>
+      <c r="WQ1" s="8"/>
+      <c r="WR1" s="8"/>
+      <c r="WS1" s="8"/>
+      <c r="WT1" s="8"/>
+      <c r="WU1" s="8"/>
+      <c r="WV1" s="8"/>
+      <c r="WW1" s="8"/>
+      <c r="WX1" s="8"/>
+      <c r="WY1" s="8"/>
+      <c r="WZ1" s="8"/>
+      <c r="XA1" s="8"/>
+      <c r="XB1" s="8"/>
+      <c r="XC1" s="8"/>
+      <c r="XD1" s="8"/>
+      <c r="XE1" s="8"/>
+      <c r="XF1" s="8"/>
+      <c r="XG1" s="8"/>
+      <c r="XH1" s="8"/>
+      <c r="XI1" s="8"/>
+      <c r="XJ1" s="8"/>
+      <c r="XK1" s="8"/>
+      <c r="XL1" s="8"/>
+      <c r="XM1" s="8"/>
+      <c r="XN1" s="8"/>
+      <c r="XO1" s="8"/>
+      <c r="XP1" s="8"/>
+      <c r="XQ1" s="8"/>
+      <c r="XR1" s="8"/>
+      <c r="XS1" s="8"/>
+      <c r="XT1" s="8"/>
+      <c r="XU1" s="8"/>
+      <c r="XV1" s="8"/>
+      <c r="XW1" s="8"/>
+      <c r="XX1" s="8"/>
+      <c r="XY1" s="8"/>
+      <c r="XZ1" s="8"/>
+      <c r="YA1" s="8"/>
+      <c r="YB1" s="8"/>
+      <c r="YC1" s="8"/>
+      <c r="YD1" s="8"/>
+      <c r="YE1" s="8"/>
+      <c r="YF1" s="8"/>
+      <c r="YG1" s="8"/>
+      <c r="YH1" s="8"/>
+      <c r="YI1" s="8"/>
+      <c r="YJ1" s="8"/>
+      <c r="YK1" s="8"/>
+      <c r="YL1" s="8"/>
+      <c r="YM1" s="8"/>
+      <c r="YN1" s="8"/>
+      <c r="YO1" s="8"/>
+      <c r="YP1" s="8"/>
+      <c r="YQ1" s="8"/>
+      <c r="YR1" s="8"/>
+      <c r="YS1" s="8"/>
+      <c r="YT1" s="8"/>
+      <c r="YU1" s="8"/>
+      <c r="YV1" s="8"/>
+      <c r="YW1" s="8"/>
+      <c r="YX1" s="8"/>
+      <c r="YY1" s="8"/>
+      <c r="YZ1" s="8"/>
+      <c r="ZA1" s="8"/>
+      <c r="ZB1" s="8"/>
+      <c r="ZC1" s="8"/>
+      <c r="ZD1" s="8"/>
+      <c r="ZE1" s="8"/>
+      <c r="ZF1" s="8"/>
+      <c r="ZG1" s="8"/>
+      <c r="ZH1" s="8"/>
+      <c r="ZI1" s="8"/>
+      <c r="ZJ1" s="8"/>
+      <c r="ZK1" s="8"/>
+      <c r="ZL1" s="8"/>
+      <c r="ZM1" s="8"/>
+      <c r="ZN1" s="8"/>
+      <c r="ZO1" s="8"/>
+      <c r="ZP1" s="8"/>
+      <c r="ZQ1" s="8"/>
+      <c r="ZR1" s="8"/>
+      <c r="ZS1" s="8"/>
+      <c r="ZT1" s="8"/>
+      <c r="ZU1" s="8"/>
+      <c r="ZV1" s="8"/>
+      <c r="ZW1" s="8"/>
+      <c r="ZX1" s="8"/>
+      <c r="ZY1" s="8"/>
+      <c r="ZZ1" s="8"/>
+      <c r="AAA1" s="8"/>
+      <c r="AAB1" s="8"/>
+      <c r="AAC1" s="8"/>
+      <c r="AAD1" s="8"/>
+      <c r="AAE1" s="8"/>
+      <c r="AAF1" s="8"/>
+      <c r="AAG1" s="8"/>
+      <c r="AAH1" s="8"/>
+      <c r="AAI1" s="8"/>
+      <c r="AAJ1" s="8"/>
+      <c r="AAK1" s="8"/>
+      <c r="AAL1" s="8"/>
+      <c r="AAM1" s="8"/>
+      <c r="AAN1" s="8"/>
+      <c r="AAO1" s="8"/>
+      <c r="AAP1" s="8"/>
+      <c r="AAQ1" s="8"/>
+      <c r="AAR1" s="8"/>
+      <c r="AAS1" s="8"/>
+      <c r="AAT1" s="8"/>
+      <c r="AAU1" s="8"/>
+      <c r="AAV1" s="8"/>
+      <c r="AAW1" s="8"/>
+      <c r="AAX1" s="8"/>
+      <c r="AAY1" s="8"/>
+      <c r="AAZ1" s="8"/>
+      <c r="ABA1" s="8"/>
+      <c r="ABB1" s="8"/>
+      <c r="ABC1" s="8"/>
+      <c r="ABD1" s="8"/>
+      <c r="ABE1" s="8"/>
+      <c r="ABF1" s="8"/>
+      <c r="ABG1" s="8"/>
+      <c r="ABH1" s="8"/>
+      <c r="ABI1" s="8"/>
+      <c r="ABJ1" s="8"/>
+      <c r="ABK1" s="8"/>
+      <c r="ABL1" s="8"/>
+      <c r="ABM1" s="8"/>
+      <c r="ABN1" s="8"/>
+      <c r="ABO1" s="8"/>
+      <c r="ABP1" s="8"/>
+      <c r="ABQ1" s="8"/>
+      <c r="ABR1" s="8"/>
+      <c r="ABS1" s="8"/>
+      <c r="ABT1" s="8"/>
+      <c r="ABU1" s="8"/>
+      <c r="ABV1" s="8"/>
+      <c r="ABW1" s="8"/>
+      <c r="ABX1" s="8"/>
+      <c r="ABY1" s="8"/>
+      <c r="ABZ1" s="8"/>
+      <c r="ACA1" s="8"/>
+      <c r="ACB1" s="8"/>
+      <c r="ACC1" s="8"/>
+      <c r="ACD1" s="8"/>
+      <c r="ACE1" s="8"/>
+      <c r="ACF1" s="8"/>
+      <c r="ACG1" s="8"/>
+      <c r="ACH1" s="8"/>
+      <c r="ACI1" s="8"/>
+      <c r="ACJ1" s="8"/>
+      <c r="ACK1" s="8"/>
+      <c r="ACL1" s="8"/>
+      <c r="ACM1" s="8"/>
+      <c r="ACN1" s="8"/>
+      <c r="ACO1" s="8"/>
+      <c r="ACP1" s="8"/>
+      <c r="ACQ1" s="8"/>
+      <c r="ACR1" s="8"/>
+      <c r="ACS1" s="8"/>
+      <c r="ACT1" s="8"/>
+      <c r="ACU1" s="8"/>
+      <c r="ACV1" s="8"/>
+      <c r="ACW1" s="8"/>
+      <c r="ACX1" s="8"/>
+      <c r="ACY1" s="8"/>
+      <c r="ACZ1" s="8"/>
+      <c r="ADA1" s="8"/>
+      <c r="ADB1" s="8"/>
+      <c r="ADC1" s="8"/>
+      <c r="ADD1" s="8"/>
+      <c r="ADE1" s="8"/>
+      <c r="ADF1" s="8"/>
+      <c r="ADG1" s="8"/>
+      <c r="ADH1" s="8"/>
+      <c r="ADI1" s="8"/>
+      <c r="ADJ1" s="8"/>
+      <c r="ADK1" s="8"/>
+      <c r="ADL1" s="8"/>
+      <c r="ADM1" s="8"/>
+      <c r="ADN1" s="8"/>
+      <c r="ADO1" s="8"/>
+      <c r="ADP1" s="8"/>
+      <c r="ADQ1" s="8"/>
+      <c r="ADR1" s="8"/>
+      <c r="ADS1" s="8"/>
+      <c r="ADT1" s="8"/>
+      <c r="ADU1" s="8"/>
+      <c r="ADV1" s="8"/>
+      <c r="ADW1" s="8"/>
+      <c r="ADX1" s="8"/>
+      <c r="ADY1" s="8"/>
+      <c r="ADZ1" s="8"/>
+      <c r="AEA1" s="8"/>
+      <c r="AEB1" s="8"/>
+      <c r="AEC1" s="8"/>
+      <c r="AED1" s="8"/>
+      <c r="AEE1" s="8"/>
+      <c r="AEF1" s="8"/>
+      <c r="AEG1" s="8"/>
+      <c r="AEH1" s="8"/>
+      <c r="AEI1" s="8"/>
+      <c r="AEJ1" s="8"/>
+      <c r="AEK1" s="8"/>
+      <c r="AEL1" s="8"/>
+      <c r="AEM1" s="8"/>
+      <c r="AEN1" s="8"/>
+      <c r="AEO1" s="8"/>
+      <c r="AEP1" s="8"/>
+      <c r="AEQ1" s="8"/>
+      <c r="AER1" s="8"/>
+      <c r="AES1" s="8"/>
+      <c r="AET1" s="8"/>
+      <c r="AEU1" s="8"/>
+      <c r="AEV1" s="8"/>
+      <c r="AEW1" s="8"/>
+      <c r="AEX1" s="8"/>
+      <c r="AEY1" s="8"/>
+      <c r="AEZ1" s="8"/>
+      <c r="AFA1" s="8"/>
+      <c r="AFB1" s="8"/>
+      <c r="AFC1" s="8"/>
+      <c r="AFD1" s="8"/>
+      <c r="AFE1" s="8"/>
+      <c r="AFF1" s="8"/>
+      <c r="AFG1" s="8"/>
+      <c r="AFH1" s="8"/>
+      <c r="AFI1" s="8"/>
+      <c r="AFJ1" s="8"/>
+      <c r="AFK1" s="8"/>
+      <c r="AFL1" s="8"/>
+      <c r="AFM1" s="8"/>
+      <c r="AFN1" s="8"/>
+      <c r="AFO1" s="8"/>
+      <c r="AFP1" s="8"/>
+      <c r="AFQ1" s="8"/>
+      <c r="AFR1" s="8"/>
+      <c r="AFS1" s="8"/>
+      <c r="AFT1" s="8"/>
+      <c r="AFU1" s="8"/>
+      <c r="AFV1" s="8"/>
+      <c r="AFW1" s="8"/>
+      <c r="AFX1" s="8"/>
+      <c r="AFY1" s="8"/>
+      <c r="AFZ1" s="8"/>
+      <c r="AGA1" s="8"/>
+      <c r="AGB1" s="8"/>
+      <c r="AGC1" s="8"/>
+      <c r="AGD1" s="8"/>
+      <c r="AGE1" s="8"/>
+      <c r="AGF1" s="8"/>
+      <c r="AGG1" s="8"/>
+      <c r="AGH1" s="8"/>
+      <c r="AGI1" s="8"/>
+      <c r="AGJ1" s="8"/>
+      <c r="AGK1" s="8"/>
+      <c r="AGL1" s="8"/>
+      <c r="AGM1" s="8"/>
+      <c r="AGN1" s="8"/>
+      <c r="AGO1" s="8"/>
+      <c r="AGP1" s="8"/>
+      <c r="AGQ1" s="8"/>
+      <c r="AGR1" s="8"/>
+      <c r="AGS1" s="8"/>
+      <c r="AGT1" s="8"/>
+      <c r="AGU1" s="8"/>
+      <c r="AGV1" s="8"/>
+      <c r="AGW1" s="8"/>
+      <c r="AGX1" s="8"/>
+      <c r="AGY1" s="8"/>
+      <c r="AGZ1" s="8"/>
+      <c r="AHA1" s="8"/>
+      <c r="AHB1" s="8"/>
+      <c r="AHC1" s="8"/>
+      <c r="AHD1" s="8"/>
+      <c r="AHE1" s="8"/>
+      <c r="AHF1" s="8"/>
+      <c r="AHG1" s="8"/>
+      <c r="AHH1" s="8"/>
+      <c r="AHI1" s="8"/>
+      <c r="AHJ1" s="8"/>
+      <c r="AHK1" s="8"/>
+      <c r="AHL1" s="8"/>
+      <c r="AHM1" s="8"/>
+      <c r="AHN1" s="8"/>
+      <c r="AHO1" s="8"/>
+      <c r="AHP1" s="8"/>
+      <c r="AHQ1" s="8"/>
+      <c r="AHR1" s="8"/>
+      <c r="AHS1" s="8"/>
+      <c r="AHT1" s="8"/>
+      <c r="AHU1" s="8"/>
+      <c r="AHV1" s="8"/>
+      <c r="AHW1" s="8"/>
+      <c r="AHX1" s="8"/>
+      <c r="AHY1" s="8"/>
+      <c r="AHZ1" s="8"/>
+      <c r="AIA1" s="8"/>
+      <c r="AIB1" s="8"/>
+      <c r="AIC1" s="8"/>
+      <c r="AID1" s="8"/>
+      <c r="AIE1" s="8"/>
+      <c r="AIF1" s="8"/>
+      <c r="AIG1" s="8"/>
+      <c r="AIH1" s="8"/>
+      <c r="AII1" s="8"/>
+      <c r="AIJ1" s="8"/>
+      <c r="AIK1" s="8"/>
+      <c r="AIL1" s="8"/>
+      <c r="AIM1" s="8"/>
+      <c r="AIN1" s="8"/>
+      <c r="AIO1" s="8"/>
+      <c r="AIP1" s="8"/>
+      <c r="AIQ1" s="8"/>
+      <c r="AIR1" s="8"/>
+      <c r="AIS1" s="8"/>
+      <c r="AIT1" s="8"/>
+      <c r="AIU1" s="8"/>
+      <c r="AIV1" s="8"/>
+      <c r="AIW1" s="8"/>
+      <c r="AIX1" s="8"/>
+      <c r="AIY1" s="8"/>
+      <c r="AIZ1" s="8"/>
+      <c r="AJA1" s="8"/>
+      <c r="AJB1" s="8"/>
+      <c r="AJC1" s="8"/>
+      <c r="AJD1" s="8"/>
+      <c r="AJE1" s="8"/>
+      <c r="AJF1" s="8"/>
+      <c r="AJG1" s="8"/>
+      <c r="AJH1" s="8"/>
+      <c r="AJI1" s="8"/>
+      <c r="AJJ1" s="8"/>
+      <c r="AJK1" s="8"/>
+      <c r="AJL1" s="8"/>
+      <c r="AJM1" s="8"/>
+      <c r="AJN1" s="8"/>
+      <c r="AJO1" s="8"/>
+      <c r="AJP1" s="8"/>
+      <c r="AJQ1" s="8"/>
+      <c r="AJR1" s="8"/>
+      <c r="AJS1" s="8"/>
+      <c r="AJT1" s="8"/>
+      <c r="AJU1" s="8"/>
+      <c r="AJV1" s="8"/>
+      <c r="AJW1" s="8"/>
+      <c r="AJX1" s="8"/>
+      <c r="AJY1" s="8"/>
+      <c r="AJZ1" s="8"/>
+      <c r="AKA1" s="8"/>
+      <c r="AKB1" s="8"/>
+      <c r="AKC1" s="8"/>
+      <c r="AKD1" s="8"/>
+      <c r="AKE1" s="8"/>
+      <c r="AKF1" s="8"/>
+      <c r="AKG1" s="8"/>
+      <c r="AKH1" s="8"/>
+      <c r="AKI1" s="8"/>
+      <c r="AKJ1" s="8"/>
+      <c r="AKK1" s="8"/>
+      <c r="AKL1" s="8"/>
+      <c r="AKM1" s="8"/>
+      <c r="AKN1" s="8"/>
+      <c r="AKO1" s="8"/>
+      <c r="AKP1" s="8"/>
+      <c r="AKQ1" s="8"/>
+      <c r="AKR1" s="8"/>
+      <c r="AKS1" s="8"/>
+      <c r="AKT1" s="8"/>
+      <c r="AKU1" s="8"/>
+      <c r="AKV1" s="8"/>
+      <c r="AKW1" s="8"/>
+      <c r="AKX1" s="8"/>
+      <c r="AKY1" s="8"/>
+      <c r="AKZ1" s="8"/>
+      <c r="ALA1" s="8"/>
+      <c r="ALB1" s="8"/>
+      <c r="ALC1" s="8"/>
+      <c r="ALD1" s="8"/>
+      <c r="ALE1" s="8"/>
+      <c r="ALF1" s="8"/>
+      <c r="ALG1" s="8"/>
+      <c r="ALH1" s="8"/>
+      <c r="ALI1" s="8"/>
+      <c r="ALJ1" s="8"/>
+      <c r="ALK1" s="8"/>
+      <c r="ALL1" s="8"/>
+      <c r="ALM1" s="8"/>
+      <c r="ALN1" s="8"/>
+      <c r="ALO1" s="8"/>
+      <c r="ALP1" s="8"/>
+      <c r="ALQ1" s="8"/>
+      <c r="ALR1" s="8"/>
+      <c r="ALS1" s="8"/>
+      <c r="ALT1" s="8"/>
+      <c r="ALU1" s="8"/>
+      <c r="ALV1" s="8"/>
+      <c r="ALW1" s="8"/>
+      <c r="ALX1" s="8"/>
+      <c r="ALY1" s="8"/>
+      <c r="ALZ1" s="8"/>
+      <c r="AMA1" s="8"/>
+      <c r="AMB1" s="8"/>
+      <c r="AMC1" s="8"/>
+      <c r="AMD1" s="8"/>
+      <c r="AME1" s="8"/>
+      <c r="AMF1" s="8"/>
+      <c r="AMG1" s="8"/>
+      <c r="AMH1" s="8"/>
+      <c r="AMI1" s="8"/>
+      <c r="AMJ1" s="8"/>
+    </row>
+    <row r="2" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>88</v>
       </c>
@@ -1731,7 +2774,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>103</v>
       </c>
@@ -1751,7 +2794,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>104</v>
       </c>
@@ -1771,7 +2814,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
@@ -1788,7 +2831,7 @@
         <v>128</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>128</v>
@@ -1809,7 +2852,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>106</v>
       </c>
@@ -1826,15 +2869,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>91</v>
@@ -1843,7 +2886,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>108</v>
       </c>
@@ -1851,10 +2894,10 @@
         <v>128</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1024" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>84</v>
       </c>
@@ -1871,27 +2914,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>129</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>132</v>
@@ -1903,18 +2946,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>111</v>
       </c>
@@ -1928,7 +2971,7 @@
         <v>130</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>130</v>
@@ -1946,12 +2989,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>85</v>
@@ -1963,12 +3006,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>85</v>
@@ -1980,30 +3023,30 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>130</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O15" s="3">
         <v>0</v>
@@ -2012,30 +3055,30 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>130</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O16" s="3">
         <v>0</v>
@@ -2049,25 +3092,25 @@
         <v>116</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>130</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O17" s="3">
         <v>0</v>
@@ -2081,25 +3124,25 @@
         <v>117</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>130</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O18" s="3">
         <v>0</v>
@@ -2134,22 +3177,22 @@
         <v>121</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>130</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O22" s="3">
         <v>0</v>

</xml_diff>